<commit_message>
Fixed book upload command
</commit_message>
<xml_diff>
--- a/book_rental/management/commands/uploads/author_upload.xlsx
+++ b/book_rental/management/commands/uploads/author_upload.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="12">
   <si>
     <t>code</t>
   </si>
@@ -105,6 +105,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="52.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -189,6 +192,426 @@
         <v>1.723987678E9</v>
       </c>
     </row>
+    <row r="5">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1.723987678E9</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>